<commit_message>
adding delta simulation for the kiko
</commit_message>
<xml_diff>
--- a/backend/test_cases.xlsx
+++ b/backend/test_cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martinfong/Study/Master/FITE7405 Techniques in computational finance/hw/CodingAssignmet/option_pricing/backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D11B88A6-F4FE-B54E-88CB-4005DA5CC866}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{271BDE0B-462A-5C48-B89D-889DF82D1BB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17700" yWindow="-21100" windowWidth="25600" windowHeight="21100" xr2:uid="{A0DFC316-593E-AF4D-B68F-A88B91C5FA7A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="30">
   <si>
     <t>r</t>
   </si>
@@ -569,11 +569,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE0A3167-F7CE-A44B-8462-655BD3DB2461}">
-  <dimension ref="A1:T82"/>
+  <dimension ref="A1:T88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K18" sqref="K18"/>
+      <selection pane="bottomLeft" activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -745,7 +745,7 @@
         <v>0.05</v>
       </c>
       <c r="C4" s="9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D4" s="9">
         <v>100</v>
@@ -763,7 +763,7 @@
         <v>100</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L4" s="9"/>
       <c r="M4" s="9"/>
@@ -789,7 +789,7 @@
         <v>100</v>
       </c>
       <c r="E5" s="9">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
@@ -798,10 +798,10 @@
         <v>0</v>
       </c>
       <c r="J5" s="9">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L5" s="9"/>
       <c r="M5" s="9"/>
@@ -813,321 +813,309 @@
       <c r="S5" s="9"/>
       <c r="T5" s="9"/>
     </row>
-    <row r="6" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
+    <row r="6" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="C6" s="9">
+        <v>3</v>
+      </c>
+      <c r="D6" s="9">
+        <v>100</v>
+      </c>
+      <c r="E6" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9">
+        <v>0</v>
+      </c>
+      <c r="J6" s="9">
+        <v>100</v>
+      </c>
+      <c r="K6" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="9"/>
+      <c r="T6" s="9"/>
+    </row>
+    <row r="7" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="C7" s="9">
+        <v>3</v>
+      </c>
+      <c r="D7" s="9">
+        <v>100</v>
+      </c>
+      <c r="E7" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9">
+        <v>0</v>
+      </c>
+      <c r="J7" s="9">
+        <v>100</v>
+      </c>
+      <c r="K7" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="9"/>
+      <c r="S7" s="9"/>
+      <c r="T7" s="9"/>
+    </row>
+    <row r="8" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="C8" s="9">
+        <v>3</v>
+      </c>
+      <c r="D8" s="9">
+        <v>100</v>
+      </c>
+      <c r="E8" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9">
+        <v>0</v>
+      </c>
+      <c r="J8" s="9">
+        <v>100</v>
+      </c>
+      <c r="K8" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="9"/>
+      <c r="S8" s="9"/>
+      <c r="T8" s="9"/>
+    </row>
+    <row r="9" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="C9" s="9">
+        <v>4</v>
+      </c>
+      <c r="D9" s="9">
+        <v>100</v>
+      </c>
+      <c r="E9" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9">
+        <v>0</v>
+      </c>
+      <c r="J9" s="9">
+        <v>100</v>
+      </c>
+      <c r="K9" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="9"/>
+      <c r="S9" s="9"/>
+      <c r="T9" s="9"/>
+    </row>
+    <row r="10" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="C10" s="9">
+        <v>3</v>
+      </c>
+      <c r="D10" s="9">
+        <v>100</v>
+      </c>
+      <c r="E10" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9">
+        <v>0</v>
+      </c>
+      <c r="J10" s="9">
+        <v>110</v>
+      </c>
+      <c r="K10" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="9"/>
+      <c r="R10" s="9"/>
+      <c r="S10" s="9"/>
+      <c r="T10" s="9"/>
+    </row>
+    <row r="11" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="C11" s="9">
+        <v>3</v>
+      </c>
+      <c r="D11" s="9">
+        <v>100</v>
+      </c>
+      <c r="E11" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9">
+        <v>0</v>
+      </c>
+      <c r="J11" s="9">
+        <v>100</v>
+      </c>
+      <c r="K11" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="9"/>
+      <c r="S11" s="9"/>
+      <c r="T11" s="9"/>
+    </row>
+    <row r="12" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="10">
-        <v>0.05</v>
-      </c>
-      <c r="C6" s="10">
-        <v>3</v>
-      </c>
-      <c r="D6" s="10">
-        <v>100</v>
-      </c>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10">
+      <c r="B12" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="C12" s="10">
+        <v>3</v>
+      </c>
+      <c r="D12" s="10">
+        <v>100</v>
+      </c>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10">
         <v>0</v>
       </c>
-      <c r="J6" s="10">
-        <v>100</v>
-      </c>
-      <c r="K6" s="10" t="s">
+      <c r="J12" s="10">
+        <v>100</v>
+      </c>
+      <c r="K12" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10">
+      <c r="L12" s="10"/>
+      <c r="M12" s="10">
         <v>12.8762812391473</v>
       </c>
-      <c r="N6" s="10"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="10"/>
-      <c r="R6" s="10"/>
-      <c r="S6" s="10"/>
-      <c r="T6" s="10"/>
-    </row>
-    <row r="7" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="10" t="s">
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="10"/>
+      <c r="R12" s="10"/>
+      <c r="S12" s="10"/>
+      <c r="T12" s="10"/>
+    </row>
+    <row r="13" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="10">
-        <v>0.05</v>
-      </c>
-      <c r="C7" s="10">
-        <v>3</v>
-      </c>
-      <c r="D7" s="10">
-        <v>100</v>
-      </c>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10">
+      <c r="B13" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="C13" s="10">
+        <v>3</v>
+      </c>
+      <c r="D13" s="10">
+        <v>100</v>
+      </c>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10">
         <v>0</v>
       </c>
-      <c r="J7" s="10">
-        <v>100</v>
-      </c>
-      <c r="K7" s="10" t="s">
+      <c r="J13" s="10">
+        <v>100</v>
+      </c>
+      <c r="K13" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10">
+      <c r="L13" s="10"/>
+      <c r="M13" s="10">
         <v>26.805483596641501</v>
       </c>
-      <c r="N7" s="10"/>
-      <c r="O7" s="10"/>
-      <c r="P7" s="10"/>
-      <c r="Q7" s="10"/>
-      <c r="R7" s="10"/>
-      <c r="S7" s="10"/>
-      <c r="T7" s="10"/>
-    </row>
-    <row r="8" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="11">
-        <v>0.05</v>
-      </c>
-      <c r="C8" s="11">
-        <v>3</v>
-      </c>
-      <c r="D8" s="11">
-        <v>100</v>
-      </c>
-      <c r="E8" s="11">
-        <v>0.3</v>
-      </c>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11">
-        <v>100</v>
-      </c>
-      <c r="K8" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="L8" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="M8" s="11"/>
-      <c r="N8" s="11">
-        <v>50</v>
-      </c>
-      <c r="O8" s="11"/>
-      <c r="P8" s="11"/>
-      <c r="Q8" s="11"/>
-      <c r="R8" s="11"/>
-      <c r="S8" s="11"/>
-      <c r="T8" s="11"/>
-    </row>
-    <row r="9" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="11">
-        <v>0.05</v>
-      </c>
-      <c r="C9" s="11">
-        <v>3</v>
-      </c>
-      <c r="D9" s="11">
-        <v>100</v>
-      </c>
-      <c r="E9" s="11">
-        <v>0.3</v>
-      </c>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11">
-        <v>100</v>
-      </c>
-      <c r="K9" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="L9" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="M9" s="11"/>
-      <c r="N9" s="11">
-        <v>100</v>
-      </c>
-      <c r="O9" s="11"/>
-      <c r="P9" s="11"/>
-      <c r="Q9" s="11"/>
-      <c r="R9" s="11"/>
-      <c r="S9" s="11"/>
-      <c r="T9" s="11"/>
-    </row>
-    <row r="10" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="11">
-        <v>0.05</v>
-      </c>
-      <c r="C10" s="11">
-        <v>3</v>
-      </c>
-      <c r="D10" s="11">
-        <v>100</v>
-      </c>
-      <c r="E10" s="11">
-        <v>0.4</v>
-      </c>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11">
-        <v>100</v>
-      </c>
-      <c r="K10" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="L10" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="M10" s="11"/>
-      <c r="N10" s="11">
-        <v>50</v>
-      </c>
-      <c r="O10" s="11"/>
-      <c r="P10" s="11"/>
-      <c r="Q10" s="11"/>
-      <c r="R10" s="11"/>
-      <c r="S10" s="11"/>
-      <c r="T10" s="11"/>
-    </row>
-    <row r="11" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="11">
-        <v>0.05</v>
-      </c>
-      <c r="C11" s="11">
-        <v>3</v>
-      </c>
-      <c r="D11" s="11">
-        <v>100</v>
-      </c>
-      <c r="E11" s="11">
-        <v>0.3</v>
-      </c>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11">
-        <v>100</v>
-      </c>
-      <c r="K11" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="L11" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="M11" s="11"/>
-      <c r="N11" s="11">
-        <v>50</v>
-      </c>
-      <c r="O11" s="11"/>
-      <c r="P11" s="11"/>
-      <c r="Q11" s="11"/>
-      <c r="R11" s="11"/>
-      <c r="S11" s="11"/>
-      <c r="T11" s="11"/>
-    </row>
-    <row r="12" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="11">
-        <v>0.05</v>
-      </c>
-      <c r="C12" s="11">
-        <v>3</v>
-      </c>
-      <c r="D12" s="11">
-        <v>100</v>
-      </c>
-      <c r="E12" s="11">
-        <v>0.3</v>
-      </c>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11">
-        <v>100</v>
-      </c>
-      <c r="K12" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="L12" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="M12" s="11"/>
-      <c r="N12" s="11">
-        <v>100</v>
-      </c>
-      <c r="O12" s="11"/>
-      <c r="P12" s="11"/>
-      <c r="Q12" s="11"/>
-      <c r="R12" s="11"/>
-      <c r="S12" s="11"/>
-      <c r="T12" s="11"/>
-    </row>
-    <row r="13" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="11">
-        <v>0.05</v>
-      </c>
-      <c r="C13" s="11">
-        <v>3</v>
-      </c>
-      <c r="D13" s="11">
-        <v>100</v>
-      </c>
-      <c r="E13" s="11">
-        <v>0.4</v>
-      </c>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11">
-        <v>100</v>
-      </c>
-      <c r="K13" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="L13" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="M13" s="11"/>
-      <c r="N13" s="11">
-        <v>50</v>
-      </c>
-      <c r="O13" s="11"/>
-      <c r="P13" s="11"/>
-      <c r="Q13" s="11"/>
-      <c r="R13" s="11"/>
-      <c r="S13" s="11"/>
-      <c r="T13" s="11"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="10"/>
+      <c r="P13" s="10"/>
+      <c r="Q13" s="10"/>
+      <c r="R13" s="10"/>
+      <c r="S13" s="10"/>
+      <c r="T13" s="10"/>
     </row>
     <row r="14" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
@@ -1156,21 +1144,15 @@
         <v>6</v>
       </c>
       <c r="L14" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M14" s="11"/>
       <c r="N14" s="11">
         <v>50</v>
       </c>
-      <c r="O14" s="11">
-        <v>100000</v>
-      </c>
-      <c r="P14" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="11" t="b">
-        <v>1</v>
-      </c>
+      <c r="O14" s="11"/>
+      <c r="P14" s="11"/>
+      <c r="Q14" s="11"/>
       <c r="R14" s="11"/>
       <c r="S14" s="11"/>
       <c r="T14" s="11"/>
@@ -1202,21 +1184,15 @@
         <v>6</v>
       </c>
       <c r="L15" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M15" s="11"/>
       <c r="N15" s="11">
         <v>100</v>
       </c>
-      <c r="O15" s="11">
-        <v>100000</v>
-      </c>
-      <c r="P15" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="11" t="b">
-        <v>1</v>
-      </c>
+      <c r="O15" s="11"/>
+      <c r="P15" s="11"/>
+      <c r="Q15" s="11"/>
       <c r="R15" s="11"/>
       <c r="S15" s="11"/>
       <c r="T15" s="11"/>
@@ -1248,21 +1224,15 @@
         <v>6</v>
       </c>
       <c r="L16" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M16" s="11"/>
       <c r="N16" s="11">
         <v>50</v>
       </c>
-      <c r="O16" s="11">
-        <v>100000</v>
-      </c>
-      <c r="P16" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="11" t="b">
-        <v>1</v>
-      </c>
+      <c r="O16" s="11"/>
+      <c r="P16" s="11"/>
+      <c r="Q16" s="11"/>
       <c r="R16" s="11"/>
       <c r="S16" s="11"/>
       <c r="T16" s="11"/>
@@ -1294,21 +1264,15 @@
         <v>7</v>
       </c>
       <c r="L17" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M17" s="11"/>
       <c r="N17" s="11">
         <v>50</v>
       </c>
-      <c r="O17" s="11">
-        <v>100000</v>
-      </c>
-      <c r="P17" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="11" t="b">
-        <v>1</v>
-      </c>
+      <c r="O17" s="11"/>
+      <c r="P17" s="11"/>
+      <c r="Q17" s="11"/>
       <c r="R17" s="11"/>
       <c r="S17" s="11"/>
       <c r="T17" s="11"/>
@@ -1340,21 +1304,15 @@
         <v>7</v>
       </c>
       <c r="L18" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M18" s="11"/>
       <c r="N18" s="11">
         <v>100</v>
       </c>
-      <c r="O18" s="11">
-        <v>100000</v>
-      </c>
-      <c r="P18" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="11" t="b">
-        <v>1</v>
-      </c>
+      <c r="O18" s="11"/>
+      <c r="P18" s="11"/>
+      <c r="Q18" s="11"/>
       <c r="R18" s="11"/>
       <c r="S18" s="11"/>
       <c r="T18" s="11"/>
@@ -1386,21 +1344,15 @@
         <v>7</v>
       </c>
       <c r="L19" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M19" s="11"/>
       <c r="N19" s="11">
         <v>50</v>
       </c>
-      <c r="O19" s="11">
-        <v>100000</v>
-      </c>
-      <c r="P19" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q19" s="11" t="b">
-        <v>1</v>
-      </c>
+      <c r="O19" s="11"/>
+      <c r="P19" s="11"/>
+      <c r="Q19" s="11"/>
       <c r="R19" s="11"/>
       <c r="S19" s="11"/>
       <c r="T19" s="11"/>
@@ -1442,7 +1394,7 @@
         <v>100000</v>
       </c>
       <c r="P20" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q20" s="11" t="b">
         <v>1</v>
@@ -1488,7 +1440,7 @@
         <v>100000</v>
       </c>
       <c r="P21" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q21" s="11" t="b">
         <v>1</v>
@@ -1534,7 +1486,7 @@
         <v>100000</v>
       </c>
       <c r="P22" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q22" s="11" t="b">
         <v>1</v>
@@ -1580,7 +1532,7 @@
         <v>100000</v>
       </c>
       <c r="P23" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q23" s="11" t="b">
         <v>1</v>
@@ -1626,7 +1578,7 @@
         <v>100000</v>
       </c>
       <c r="P24" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q24" s="11" t="b">
         <v>1</v>
@@ -1672,7 +1624,7 @@
         <v>100000</v>
       </c>
       <c r="P25" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q25" s="11" t="b">
         <v>1</v>
@@ -1681,269 +1633,281 @@
       <c r="S25" s="11"/>
       <c r="T25" s="11"/>
     </row>
-    <row r="26" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B26" s="12">
-        <v>0.05</v>
-      </c>
-      <c r="C26" s="12">
-        <v>3</v>
-      </c>
-      <c r="D26" s="12">
-        <v>100</v>
-      </c>
-      <c r="E26" s="12">
-        <v>0.3</v>
-      </c>
-      <c r="F26" s="12">
-        <v>100</v>
-      </c>
-      <c r="G26" s="12">
-        <v>0.3</v>
-      </c>
-      <c r="H26" s="12">
-        <v>0.5</v>
-      </c>
-      <c r="I26" s="12"/>
-      <c r="J26" s="12">
-        <v>100</v>
-      </c>
-      <c r="K26" s="12" t="s">
+    <row r="26" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="C26" s="11">
+        <v>3</v>
+      </c>
+      <c r="D26" s="11">
+        <v>100</v>
+      </c>
+      <c r="E26" s="11">
+        <v>0.3</v>
+      </c>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11">
+        <v>100</v>
+      </c>
+      <c r="K26" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="L26" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="M26" s="12"/>
-      <c r="N26" s="12"/>
-      <c r="O26" s="12"/>
-      <c r="P26" s="12"/>
-      <c r="Q26" s="12"/>
-      <c r="R26" s="12"/>
-      <c r="S26" s="12"/>
-      <c r="T26" s="12"/>
-    </row>
-    <row r="27" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B27" s="12">
-        <v>0.05</v>
-      </c>
-      <c r="C27" s="12">
-        <v>3</v>
-      </c>
-      <c r="D27" s="12">
-        <v>100</v>
-      </c>
-      <c r="E27" s="12">
-        <v>0.3</v>
-      </c>
-      <c r="F27" s="12">
-        <v>100</v>
-      </c>
-      <c r="G27" s="12">
-        <v>0.3</v>
-      </c>
-      <c r="H27" s="12">
-        <v>0.9</v>
-      </c>
-      <c r="I27" s="12"/>
-      <c r="J27" s="12">
-        <v>100</v>
-      </c>
-      <c r="K27" s="12" t="s">
+      <c r="L26" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="M26" s="11"/>
+      <c r="N26" s="11">
+        <v>50</v>
+      </c>
+      <c r="O26" s="11">
+        <v>100000</v>
+      </c>
+      <c r="P26" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q26" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="R26" s="11"/>
+      <c r="S26" s="11"/>
+      <c r="T26" s="11"/>
+    </row>
+    <row r="27" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="C27" s="11">
+        <v>3</v>
+      </c>
+      <c r="D27" s="11">
+        <v>100</v>
+      </c>
+      <c r="E27" s="11">
+        <v>0.3</v>
+      </c>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="11">
+        <v>100</v>
+      </c>
+      <c r="K27" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="L27" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="M27" s="12"/>
-      <c r="N27" s="12"/>
-      <c r="O27" s="12"/>
-      <c r="P27" s="12"/>
-      <c r="Q27" s="12"/>
-      <c r="R27" s="12"/>
-      <c r="S27" s="12"/>
-      <c r="T27" s="12"/>
-    </row>
-    <row r="28" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B28" s="12">
-        <v>0.05</v>
-      </c>
-      <c r="C28" s="12">
-        <v>3</v>
-      </c>
-      <c r="D28" s="12">
-        <v>100</v>
-      </c>
-      <c r="E28" s="12">
-        <v>0.1</v>
-      </c>
-      <c r="F28" s="12">
-        <v>100</v>
-      </c>
-      <c r="G28" s="12">
-        <v>0.3</v>
-      </c>
-      <c r="H28" s="12">
-        <v>0.5</v>
-      </c>
-      <c r="I28" s="12"/>
-      <c r="J28" s="12">
-        <v>100</v>
-      </c>
-      <c r="K28" s="12" t="s">
+      <c r="L27" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="M27" s="11"/>
+      <c r="N27" s="11">
+        <v>100</v>
+      </c>
+      <c r="O27" s="11">
+        <v>100000</v>
+      </c>
+      <c r="P27" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q27" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="R27" s="11"/>
+      <c r="S27" s="11"/>
+      <c r="T27" s="11"/>
+    </row>
+    <row r="28" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="C28" s="11">
+        <v>3</v>
+      </c>
+      <c r="D28" s="11">
+        <v>100</v>
+      </c>
+      <c r="E28" s="11">
+        <v>0.4</v>
+      </c>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="11">
+        <v>100</v>
+      </c>
+      <c r="K28" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="L28" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="M28" s="12"/>
-      <c r="N28" s="12"/>
-      <c r="O28" s="12"/>
-      <c r="P28" s="12"/>
-      <c r="Q28" s="12"/>
-      <c r="R28" s="12"/>
-      <c r="S28" s="12"/>
-      <c r="T28" s="12"/>
-    </row>
-    <row r="29" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B29" s="12">
-        <v>0.05</v>
-      </c>
-      <c r="C29" s="12">
-        <v>3</v>
-      </c>
-      <c r="D29" s="12">
-        <v>100</v>
-      </c>
-      <c r="E29" s="12">
-        <v>0.3</v>
-      </c>
-      <c r="F29" s="12">
-        <v>100</v>
-      </c>
-      <c r="G29" s="12">
-        <v>0.3</v>
-      </c>
-      <c r="H29" s="12">
-        <v>0.5</v>
-      </c>
-      <c r="I29" s="12"/>
-      <c r="J29" s="12">
-        <v>80</v>
-      </c>
-      <c r="K29" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="L29" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="M29" s="12"/>
-      <c r="N29" s="12"/>
-      <c r="O29" s="12"/>
-      <c r="P29" s="12"/>
-      <c r="Q29" s="12"/>
-      <c r="R29" s="12"/>
-      <c r="S29" s="12"/>
-      <c r="T29" s="12"/>
-    </row>
-    <row r="30" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B30" s="12">
-        <v>0.05</v>
-      </c>
-      <c r="C30" s="12">
-        <v>3</v>
-      </c>
-      <c r="D30" s="12">
-        <v>100</v>
-      </c>
-      <c r="E30" s="12">
-        <v>0.3</v>
-      </c>
-      <c r="F30" s="12">
-        <v>100</v>
-      </c>
-      <c r="G30" s="12">
-        <v>0.3</v>
-      </c>
-      <c r="H30" s="12">
-        <v>0.5</v>
-      </c>
-      <c r="I30" s="12"/>
-      <c r="J30" s="12">
-        <v>120</v>
-      </c>
-      <c r="K30" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="L30" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="M30" s="12"/>
-      <c r="N30" s="12"/>
-      <c r="O30" s="12"/>
-      <c r="P30" s="12"/>
-      <c r="Q30" s="12"/>
-      <c r="R30" s="12"/>
-      <c r="S30" s="12"/>
-      <c r="T30" s="12"/>
-    </row>
-    <row r="31" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B31" s="12">
-        <v>0.05</v>
-      </c>
-      <c r="C31" s="12">
-        <v>3</v>
-      </c>
-      <c r="D31" s="12">
-        <v>100</v>
-      </c>
-      <c r="E31" s="12">
-        <v>0.5</v>
-      </c>
-      <c r="F31" s="12">
-        <v>100</v>
-      </c>
-      <c r="G31" s="12">
-        <v>0.5</v>
-      </c>
-      <c r="H31" s="12">
-        <v>0.5</v>
-      </c>
-      <c r="I31" s="12"/>
-      <c r="J31" s="12">
-        <v>100</v>
-      </c>
-      <c r="K31" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="L31" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="M31" s="12"/>
-      <c r="N31" s="12"/>
-      <c r="O31" s="12"/>
-      <c r="P31" s="12"/>
-      <c r="Q31" s="12"/>
-      <c r="R31" s="12"/>
-      <c r="S31" s="12"/>
-      <c r="T31" s="12"/>
+      <c r="L28" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="M28" s="11"/>
+      <c r="N28" s="11">
+        <v>50</v>
+      </c>
+      <c r="O28" s="11">
+        <v>100000</v>
+      </c>
+      <c r="P28" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q28" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="R28" s="11"/>
+      <c r="S28" s="11"/>
+      <c r="T28" s="11"/>
+    </row>
+    <row r="29" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="C29" s="11">
+        <v>3</v>
+      </c>
+      <c r="D29" s="11">
+        <v>100</v>
+      </c>
+      <c r="E29" s="11">
+        <v>0.3</v>
+      </c>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="11">
+        <v>100</v>
+      </c>
+      <c r="K29" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="L29" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="M29" s="11"/>
+      <c r="N29" s="11">
+        <v>50</v>
+      </c>
+      <c r="O29" s="11">
+        <v>100000</v>
+      </c>
+      <c r="P29" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q29" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="R29" s="11"/>
+      <c r="S29" s="11"/>
+      <c r="T29" s="11"/>
+    </row>
+    <row r="30" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="C30" s="11">
+        <v>3</v>
+      </c>
+      <c r="D30" s="11">
+        <v>100</v>
+      </c>
+      <c r="E30" s="11">
+        <v>0.3</v>
+      </c>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="11">
+        <v>100</v>
+      </c>
+      <c r="K30" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="L30" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="M30" s="11"/>
+      <c r="N30" s="11">
+        <v>100</v>
+      </c>
+      <c r="O30" s="11">
+        <v>100000</v>
+      </c>
+      <c r="P30" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q30" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="R30" s="11"/>
+      <c r="S30" s="11"/>
+      <c r="T30" s="11"/>
+    </row>
+    <row r="31" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B31" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="C31" s="11">
+        <v>3</v>
+      </c>
+      <c r="D31" s="11">
+        <v>100</v>
+      </c>
+      <c r="E31" s="11">
+        <v>0.4</v>
+      </c>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="11">
+        <v>100</v>
+      </c>
+      <c r="K31" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="L31" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="M31" s="11"/>
+      <c r="N31" s="11">
+        <v>50</v>
+      </c>
+      <c r="O31" s="11">
+        <v>100000</v>
+      </c>
+      <c r="P31" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q31" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="R31" s="11"/>
+      <c r="S31" s="11"/>
+      <c r="T31" s="11"/>
     </row>
     <row r="32" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="12" t="s">
@@ -1975,7 +1939,7 @@
         <v>100</v>
       </c>
       <c r="K32" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L32" s="12" t="s">
         <v>17</v>
@@ -2019,7 +1983,7 @@
         <v>100</v>
       </c>
       <c r="K33" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L33" s="12" t="s">
         <v>17</v>
@@ -2063,7 +2027,7 @@
         <v>100</v>
       </c>
       <c r="K34" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L34" s="12" t="s">
         <v>17</v>
@@ -2107,7 +2071,7 @@
         <v>80</v>
       </c>
       <c r="K35" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L35" s="12" t="s">
         <v>17</v>
@@ -2151,7 +2115,7 @@
         <v>120</v>
       </c>
       <c r="K36" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L36" s="12" t="s">
         <v>17</v>
@@ -2195,7 +2159,7 @@
         <v>100</v>
       </c>
       <c r="K37" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L37" s="12" t="s">
         <v>17</v>
@@ -2239,22 +2203,16 @@
         <v>100</v>
       </c>
       <c r="K38" s="12" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L38" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M38" s="12"/>
       <c r="N38" s="12"/>
-      <c r="O38" s="12">
-        <v>100000</v>
-      </c>
-      <c r="P38" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q38" s="12" t="b">
-        <v>1</v>
-      </c>
+      <c r="O38" s="12"/>
+      <c r="P38" s="12"/>
+      <c r="Q38" s="12"/>
       <c r="R38" s="12"/>
       <c r="S38" s="12"/>
       <c r="T38" s="12"/>
@@ -2289,22 +2247,16 @@
         <v>100</v>
       </c>
       <c r="K39" s="12" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L39" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M39" s="12"/>
       <c r="N39" s="12"/>
-      <c r="O39" s="12">
-        <v>100000</v>
-      </c>
-      <c r="P39" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q39" s="12" t="b">
-        <v>1</v>
-      </c>
+      <c r="O39" s="12"/>
+      <c r="P39" s="12"/>
+      <c r="Q39" s="12"/>
       <c r="R39" s="12"/>
       <c r="S39" s="12"/>
       <c r="T39" s="12"/>
@@ -2339,22 +2291,16 @@
         <v>100</v>
       </c>
       <c r="K40" s="12" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L40" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M40" s="12"/>
       <c r="N40" s="12"/>
-      <c r="O40" s="12">
-        <v>100000</v>
-      </c>
-      <c r="P40" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q40" s="12" t="b">
-        <v>1</v>
-      </c>
+      <c r="O40" s="12"/>
+      <c r="P40" s="12"/>
+      <c r="Q40" s="12"/>
       <c r="R40" s="12"/>
       <c r="S40" s="12"/>
       <c r="T40" s="12"/>
@@ -2389,22 +2335,16 @@
         <v>80</v>
       </c>
       <c r="K41" s="12" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L41" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M41" s="12"/>
       <c r="N41" s="12"/>
-      <c r="O41" s="12">
-        <v>100000</v>
-      </c>
-      <c r="P41" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q41" s="12" t="b">
-        <v>1</v>
-      </c>
+      <c r="O41" s="12"/>
+      <c r="P41" s="12"/>
+      <c r="Q41" s="12"/>
       <c r="R41" s="12"/>
       <c r="S41" s="12"/>
       <c r="T41" s="12"/>
@@ -2439,22 +2379,16 @@
         <v>120</v>
       </c>
       <c r="K42" s="12" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L42" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M42" s="12"/>
       <c r="N42" s="12"/>
-      <c r="O42" s="12">
-        <v>100000</v>
-      </c>
-      <c r="P42" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q42" s="12" t="b">
-        <v>1</v>
-      </c>
+      <c r="O42" s="12"/>
+      <c r="P42" s="12"/>
+      <c r="Q42" s="12"/>
       <c r="R42" s="12"/>
       <c r="S42" s="12"/>
       <c r="T42" s="12"/>
@@ -2489,22 +2423,16 @@
         <v>100</v>
       </c>
       <c r="K43" s="12" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L43" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M43" s="12"/>
       <c r="N43" s="12"/>
-      <c r="O43" s="12">
-        <v>100000</v>
-      </c>
-      <c r="P43" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q43" s="12" t="b">
-        <v>1</v>
-      </c>
+      <c r="O43" s="12"/>
+      <c r="P43" s="12"/>
+      <c r="Q43" s="12"/>
       <c r="R43" s="12"/>
       <c r="S43" s="12"/>
       <c r="T43" s="12"/>
@@ -2539,7 +2467,7 @@
         <v>100</v>
       </c>
       <c r="K44" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L44" s="12" t="s">
         <v>18</v>
@@ -2589,7 +2517,7 @@
         <v>100</v>
       </c>
       <c r="K45" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L45" s="12" t="s">
         <v>18</v>
@@ -2639,7 +2567,7 @@
         <v>100</v>
       </c>
       <c r="K46" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L46" s="12" t="s">
         <v>18</v>
@@ -2689,7 +2617,7 @@
         <v>80</v>
       </c>
       <c r="K47" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L47" s="12" t="s">
         <v>18</v>
@@ -2739,7 +2667,7 @@
         <v>120</v>
       </c>
       <c r="K48" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L48" s="12" t="s">
         <v>18</v>
@@ -2789,7 +2717,7 @@
         <v>100</v>
       </c>
       <c r="K49" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L49" s="12" t="s">
         <v>18</v>
@@ -2839,7 +2767,7 @@
         <v>100</v>
       </c>
       <c r="K50" s="12" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L50" s="12" t="s">
         <v>18</v>
@@ -2850,7 +2778,7 @@
         <v>100000</v>
       </c>
       <c r="P50" s="12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q50" s="12" t="b">
         <v>1</v>
@@ -2889,7 +2817,7 @@
         <v>100</v>
       </c>
       <c r="K51" s="12" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L51" s="12" t="s">
         <v>18</v>
@@ -2900,7 +2828,7 @@
         <v>100000</v>
       </c>
       <c r="P51" s="12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q51" s="12" t="b">
         <v>1</v>
@@ -2939,7 +2867,7 @@
         <v>100</v>
       </c>
       <c r="K52" s="12" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L52" s="12" t="s">
         <v>18</v>
@@ -2950,7 +2878,7 @@
         <v>100000</v>
       </c>
       <c r="P52" s="12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q52" s="12" t="b">
         <v>1</v>
@@ -2989,7 +2917,7 @@
         <v>80</v>
       </c>
       <c r="K53" s="12" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L53" s="12" t="s">
         <v>18</v>
@@ -3000,7 +2928,7 @@
         <v>100000</v>
       </c>
       <c r="P53" s="12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q53" s="12" t="b">
         <v>1</v>
@@ -3039,7 +2967,7 @@
         <v>120</v>
       </c>
       <c r="K54" s="12" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L54" s="12" t="s">
         <v>18</v>
@@ -3050,7 +2978,7 @@
         <v>100000</v>
       </c>
       <c r="P54" s="12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q54" s="12" t="b">
         <v>1</v>
@@ -3100,7 +3028,7 @@
         <v>100000</v>
       </c>
       <c r="P55" s="12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q55" s="12" t="b">
         <v>1</v>
@@ -3139,7 +3067,7 @@
         <v>100</v>
       </c>
       <c r="K56" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L56" s="12" t="s">
         <v>18</v>
@@ -3189,7 +3117,7 @@
         <v>100</v>
       </c>
       <c r="K57" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L57" s="12" t="s">
         <v>18</v>
@@ -3239,7 +3167,7 @@
         <v>100</v>
       </c>
       <c r="K58" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L58" s="12" t="s">
         <v>18</v>
@@ -3289,7 +3217,7 @@
         <v>80</v>
       </c>
       <c r="K59" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L59" s="12" t="s">
         <v>18</v>
@@ -3339,7 +3267,7 @@
         <v>120</v>
       </c>
       <c r="K60" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L60" s="12" t="s">
         <v>18</v>
@@ -3409,479 +3337,507 @@
       <c r="S61" s="12"/>
       <c r="T61" s="12"/>
     </row>
-    <row r="62" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="13" t="s">
+    <row r="62" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B62" s="12">
+        <v>0.05</v>
+      </c>
+      <c r="C62" s="12">
+        <v>3</v>
+      </c>
+      <c r="D62" s="12">
+        <v>100</v>
+      </c>
+      <c r="E62" s="12">
+        <v>0.3</v>
+      </c>
+      <c r="F62" s="12">
+        <v>100</v>
+      </c>
+      <c r="G62" s="12">
+        <v>0.3</v>
+      </c>
+      <c r="H62" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="I62" s="12"/>
+      <c r="J62" s="12">
+        <v>100</v>
+      </c>
+      <c r="K62" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="L62" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="M62" s="12"/>
+      <c r="N62" s="12"/>
+      <c r="O62" s="12">
+        <v>100000</v>
+      </c>
+      <c r="P62" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q62" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="R62" s="12"/>
+      <c r="S62" s="12"/>
+      <c r="T62" s="12"/>
+    </row>
+    <row r="63" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B63" s="12">
+        <v>0.05</v>
+      </c>
+      <c r="C63" s="12">
+        <v>3</v>
+      </c>
+      <c r="D63" s="12">
+        <v>100</v>
+      </c>
+      <c r="E63" s="12">
+        <v>0.3</v>
+      </c>
+      <c r="F63" s="12">
+        <v>100</v>
+      </c>
+      <c r="G63" s="12">
+        <v>0.3</v>
+      </c>
+      <c r="H63" s="12">
+        <v>0.9</v>
+      </c>
+      <c r="I63" s="12"/>
+      <c r="J63" s="12">
+        <v>100</v>
+      </c>
+      <c r="K63" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="L63" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="M63" s="12"/>
+      <c r="N63" s="12"/>
+      <c r="O63" s="12">
+        <v>100000</v>
+      </c>
+      <c r="P63" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q63" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="R63" s="12"/>
+      <c r="S63" s="12"/>
+      <c r="T63" s="12"/>
+    </row>
+    <row r="64" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B64" s="12">
+        <v>0.05</v>
+      </c>
+      <c r="C64" s="12">
+        <v>3</v>
+      </c>
+      <c r="D64" s="12">
+        <v>100</v>
+      </c>
+      <c r="E64" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="F64" s="12">
+        <v>100</v>
+      </c>
+      <c r="G64" s="12">
+        <v>0.3</v>
+      </c>
+      <c r="H64" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="I64" s="12"/>
+      <c r="J64" s="12">
+        <v>100</v>
+      </c>
+      <c r="K64" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="L64" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="M64" s="12"/>
+      <c r="N64" s="12"/>
+      <c r="O64" s="12">
+        <v>100000</v>
+      </c>
+      <c r="P64" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q64" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="R64" s="12"/>
+      <c r="S64" s="12"/>
+      <c r="T64" s="12"/>
+    </row>
+    <row r="65" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B65" s="12">
+        <v>0.05</v>
+      </c>
+      <c r="C65" s="12">
+        <v>3</v>
+      </c>
+      <c r="D65" s="12">
+        <v>100</v>
+      </c>
+      <c r="E65" s="12">
+        <v>0.3</v>
+      </c>
+      <c r="F65" s="12">
+        <v>100</v>
+      </c>
+      <c r="G65" s="12">
+        <v>0.3</v>
+      </c>
+      <c r="H65" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="I65" s="12"/>
+      <c r="J65" s="12">
+        <v>80</v>
+      </c>
+      <c r="K65" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="L65" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="M65" s="12"/>
+      <c r="N65" s="12"/>
+      <c r="O65" s="12">
+        <v>100000</v>
+      </c>
+      <c r="P65" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q65" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="R65" s="12"/>
+      <c r="S65" s="12"/>
+      <c r="T65" s="12"/>
+    </row>
+    <row r="66" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B66" s="12">
+        <v>0.05</v>
+      </c>
+      <c r="C66" s="12">
+        <v>3</v>
+      </c>
+      <c r="D66" s="12">
+        <v>100</v>
+      </c>
+      <c r="E66" s="12">
+        <v>0.3</v>
+      </c>
+      <c r="F66" s="12">
+        <v>100</v>
+      </c>
+      <c r="G66" s="12">
+        <v>0.3</v>
+      </c>
+      <c r="H66" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="I66" s="12"/>
+      <c r="J66" s="12">
+        <v>120</v>
+      </c>
+      <c r="K66" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="L66" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="M66" s="12"/>
+      <c r="N66" s="12"/>
+      <c r="O66" s="12">
+        <v>100000</v>
+      </c>
+      <c r="P66" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q66" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="R66" s="12"/>
+      <c r="S66" s="12"/>
+      <c r="T66" s="12"/>
+    </row>
+    <row r="67" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B67" s="12">
+        <v>0.05</v>
+      </c>
+      <c r="C67" s="12">
+        <v>3</v>
+      </c>
+      <c r="D67" s="12">
+        <v>100</v>
+      </c>
+      <c r="E67" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="F67" s="12">
+        <v>100</v>
+      </c>
+      <c r="G67" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="H67" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="I67" s="12"/>
+      <c r="J67" s="12">
+        <v>100</v>
+      </c>
+      <c r="K67" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="L67" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="M67" s="12"/>
+      <c r="N67" s="12"/>
+      <c r="O67" s="12">
+        <v>100000</v>
+      </c>
+      <c r="P67" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q67" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="R67" s="12"/>
+      <c r="S67" s="12"/>
+      <c r="T67" s="12"/>
+    </row>
+    <row r="68" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B62" s="13">
-        <v>0.05</v>
-      </c>
-      <c r="C62" s="13">
-        <v>3</v>
-      </c>
-      <c r="D62" s="13">
-        <v>100</v>
-      </c>
-      <c r="E62" s="13">
-        <v>0.3</v>
-      </c>
-      <c r="F62" s="13"/>
-      <c r="G62" s="13"/>
-      <c r="H62" s="13"/>
-      <c r="I62" s="13"/>
-      <c r="J62" s="13">
-        <v>100</v>
-      </c>
-      <c r="K62" s="13" t="s">
+      <c r="B68" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="C68" s="13">
+        <v>3</v>
+      </c>
+      <c r="D68" s="13">
+        <v>100</v>
+      </c>
+      <c r="E68" s="13">
+        <v>0.3</v>
+      </c>
+      <c r="F68" s="13"/>
+      <c r="G68" s="13"/>
+      <c r="H68" s="13"/>
+      <c r="I68" s="13"/>
+      <c r="J68" s="13">
+        <v>100</v>
+      </c>
+      <c r="K68" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="L62" s="13"/>
-      <c r="M62" s="13"/>
-      <c r="N62" s="13">
+      <c r="L68" s="13"/>
+      <c r="M68" s="13"/>
+      <c r="N68" s="13">
         <v>200</v>
       </c>
-      <c r="O62" s="13"/>
-      <c r="P62" s="13"/>
-      <c r="Q62" s="13"/>
-      <c r="R62" s="13"/>
-      <c r="S62" s="13"/>
-      <c r="T62" s="13"/>
-    </row>
-    <row r="63" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="13" t="s">
+      <c r="O68" s="13"/>
+      <c r="P68" s="13"/>
+      <c r="Q68" s="13"/>
+      <c r="R68" s="13"/>
+      <c r="S68" s="13"/>
+      <c r="T68" s="13"/>
+    </row>
+    <row r="69" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B63" s="13">
-        <v>0.05</v>
-      </c>
-      <c r="C63" s="13">
-        <v>3</v>
-      </c>
-      <c r="D63" s="13">
-        <v>100</v>
-      </c>
-      <c r="E63" s="13">
+      <c r="B69" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="C69" s="13">
+        <v>3</v>
+      </c>
+      <c r="D69" s="13">
+        <v>100</v>
+      </c>
+      <c r="E69" s="13">
         <v>0.4</v>
       </c>
-      <c r="F63" s="13"/>
-      <c r="G63" s="13"/>
-      <c r="H63" s="13"/>
-      <c r="I63" s="13"/>
-      <c r="J63" s="13">
-        <v>100</v>
-      </c>
-      <c r="K63" s="13" t="s">
+      <c r="F69" s="13"/>
+      <c r="G69" s="13"/>
+      <c r="H69" s="13"/>
+      <c r="I69" s="13"/>
+      <c r="J69" s="13">
+        <v>100</v>
+      </c>
+      <c r="K69" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="L63" s="13"/>
-      <c r="M63" s="13"/>
-      <c r="N63" s="13">
+      <c r="L69" s="13"/>
+      <c r="M69" s="13"/>
+      <c r="N69" s="13">
         <v>200</v>
       </c>
-      <c r="O63" s="13"/>
-      <c r="P63" s="13"/>
-      <c r="Q63" s="13"/>
-      <c r="R63" s="13"/>
-      <c r="S63" s="13"/>
-      <c r="T63" s="13"/>
-    </row>
-    <row r="64" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="13" t="s">
+      <c r="O69" s="13"/>
+      <c r="P69" s="13"/>
+      <c r="Q69" s="13"/>
+      <c r="R69" s="13"/>
+      <c r="S69" s="13"/>
+      <c r="T69" s="13"/>
+    </row>
+    <row r="70" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B64" s="13">
-        <v>0.05</v>
-      </c>
-      <c r="C64" s="13">
-        <v>3</v>
-      </c>
-      <c r="D64" s="13">
-        <v>100</v>
-      </c>
-      <c r="E64" s="13">
-        <v>0.3</v>
-      </c>
-      <c r="F64" s="13"/>
-      <c r="G64" s="13"/>
-      <c r="H64" s="13"/>
-      <c r="I64" s="13"/>
-      <c r="J64" s="13">
-        <v>100</v>
-      </c>
-      <c r="K64" s="13" t="s">
+      <c r="B70" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="C70" s="13">
+        <v>3</v>
+      </c>
+      <c r="D70" s="13">
+        <v>100</v>
+      </c>
+      <c r="E70" s="13">
+        <v>0.3</v>
+      </c>
+      <c r="F70" s="13"/>
+      <c r="G70" s="13"/>
+      <c r="H70" s="13"/>
+      <c r="I70" s="13"/>
+      <c r="J70" s="13">
+        <v>100</v>
+      </c>
+      <c r="K70" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="L64" s="13"/>
-      <c r="M64" s="13"/>
-      <c r="N64" s="13">
+      <c r="L70" s="13"/>
+      <c r="M70" s="13"/>
+      <c r="N70" s="13">
         <v>200</v>
       </c>
-      <c r="O64" s="13"/>
-      <c r="P64" s="13"/>
-      <c r="Q64" s="13"/>
-      <c r="R64" s="13"/>
-      <c r="S64" s="13"/>
-      <c r="T64" s="13"/>
-    </row>
-    <row r="65" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="13" t="s">
+      <c r="O70" s="13"/>
+      <c r="P70" s="13"/>
+      <c r="Q70" s="13"/>
+      <c r="R70" s="13"/>
+      <c r="S70" s="13"/>
+      <c r="T70" s="13"/>
+    </row>
+    <row r="71" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B65" s="13">
-        <v>0.05</v>
-      </c>
-      <c r="C65" s="13">
-        <v>3</v>
-      </c>
-      <c r="D65" s="13">
-        <v>100</v>
-      </c>
-      <c r="E65" s="13">
+      <c r="B71" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="C71" s="13">
+        <v>3</v>
+      </c>
+      <c r="D71" s="13">
+        <v>100</v>
+      </c>
+      <c r="E71" s="13">
         <v>0.4</v>
       </c>
-      <c r="F65" s="13"/>
-      <c r="G65" s="13"/>
-      <c r="H65" s="13"/>
-      <c r="I65" s="13"/>
-      <c r="J65" s="13">
-        <v>100</v>
-      </c>
-      <c r="K65" s="13" t="s">
+      <c r="F71" s="13"/>
+      <c r="G71" s="13"/>
+      <c r="H71" s="13"/>
+      <c r="I71" s="13"/>
+      <c r="J71" s="13">
+        <v>100</v>
+      </c>
+      <c r="K71" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="L65" s="13"/>
-      <c r="M65" s="13"/>
-      <c r="N65" s="13">
+      <c r="L71" s="13"/>
+      <c r="M71" s="13"/>
+      <c r="N71" s="13">
         <v>200</v>
       </c>
-      <c r="O65" s="13"/>
-      <c r="P65" s="13"/>
-      <c r="Q65" s="13"/>
-      <c r="R65" s="13"/>
-      <c r="S65" s="13"/>
-      <c r="T65" s="13"/>
-    </row>
-    <row r="66" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="14" t="s">
+      <c r="O71" s="13"/>
+      <c r="P71" s="13"/>
+      <c r="Q71" s="13"/>
+      <c r="R71" s="13"/>
+      <c r="S71" s="13"/>
+      <c r="T71" s="13"/>
+    </row>
+    <row r="72" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B66" s="14">
-        <v>0.05</v>
-      </c>
-      <c r="C66" s="14">
-        <v>3</v>
-      </c>
-      <c r="D66" s="14">
-        <v>100</v>
-      </c>
-      <c r="E66" s="14">
-        <v>0.3</v>
-      </c>
-      <c r="F66" s="14"/>
-      <c r="G66" s="14"/>
-      <c r="H66" s="14"/>
-      <c r="I66" s="14"/>
-      <c r="J66" s="14">
-        <v>100</v>
-      </c>
-      <c r="K66" s="14" t="s">
+      <c r="B72" s="14">
+        <v>0.05</v>
+      </c>
+      <c r="C72" s="14">
+        <v>3</v>
+      </c>
+      <c r="D72" s="14">
+        <v>100</v>
+      </c>
+      <c r="E72" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="F72" s="14"/>
+      <c r="G72" s="14"/>
+      <c r="H72" s="14"/>
+      <c r="I72" s="14"/>
+      <c r="J72" s="14">
+        <v>100</v>
+      </c>
+      <c r="K72" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="L66" s="14"/>
-      <c r="M66" s="14"/>
-      <c r="N66" s="14">
+      <c r="L72" s="14"/>
+      <c r="M72" s="14"/>
+      <c r="N72" s="14">
         <v>36</v>
       </c>
-      <c r="O66" s="14">
-        <v>100000</v>
-      </c>
-      <c r="P66" s="14"/>
-      <c r="Q66" s="14"/>
-      <c r="R66" s="14">
+      <c r="O72" s="14">
+        <v>100000</v>
+      </c>
+      <c r="P72" s="14"/>
+      <c r="Q72" s="14"/>
+      <c r="R72" s="14">
         <v>80</v>
       </c>
-      <c r="S66" s="14">
+      <c r="S72" s="14">
         <v>125</v>
       </c>
-      <c r="T66" s="14">
+      <c r="T72" s="14">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="67" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="B67" s="15">
-        <v>0.05</v>
-      </c>
-      <c r="C67" s="15">
-        <v>3</v>
-      </c>
-      <c r="D67" s="15">
-        <v>100</v>
-      </c>
-      <c r="E67" s="15">
-        <v>0.3</v>
-      </c>
-      <c r="F67" s="15"/>
-      <c r="G67" s="15"/>
-      <c r="H67" s="15"/>
-      <c r="I67" s="15"/>
-      <c r="J67" s="15">
-        <v>100</v>
-      </c>
-      <c r="K67" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="L67" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="M67" s="15"/>
-      <c r="N67" s="15">
-        <v>50</v>
-      </c>
-      <c r="O67" s="15">
-        <v>100000</v>
-      </c>
-      <c r="P67" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q67" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="R67" s="15"/>
-      <c r="S67" s="15"/>
-      <c r="T67" s="15"/>
-    </row>
-    <row r="68" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="B68" s="15">
-        <v>0.05</v>
-      </c>
-      <c r="C68" s="15">
-        <v>3</v>
-      </c>
-      <c r="D68" s="15">
-        <v>100</v>
-      </c>
-      <c r="E68" s="15">
-        <v>0.3</v>
-      </c>
-      <c r="F68" s="15"/>
-      <c r="G68" s="15"/>
-      <c r="H68" s="15"/>
-      <c r="I68" s="15"/>
-      <c r="J68" s="15">
-        <v>100</v>
-      </c>
-      <c r="K68" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="L68" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="M68" s="15"/>
-      <c r="N68" s="15">
-        <v>50</v>
-      </c>
-      <c r="O68" s="15">
-        <v>100000</v>
-      </c>
-      <c r="P68" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q68" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="R68" s="15"/>
-      <c r="S68" s="15"/>
-      <c r="T68" s="15"/>
-    </row>
-    <row r="69" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="B69" s="15">
-        <v>0.05</v>
-      </c>
-      <c r="C69" s="15">
-        <v>3</v>
-      </c>
-      <c r="D69" s="15">
-        <v>100</v>
-      </c>
-      <c r="E69" s="15">
-        <v>0.3</v>
-      </c>
-      <c r="F69" s="15"/>
-      <c r="G69" s="15"/>
-      <c r="H69" s="15"/>
-      <c r="I69" s="15"/>
-      <c r="J69" s="15">
-        <v>100</v>
-      </c>
-      <c r="K69" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="L69" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="M69" s="15"/>
-      <c r="N69" s="15">
-        <v>50</v>
-      </c>
-      <c r="O69" s="15">
-        <v>100000</v>
-      </c>
-      <c r="P69" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q69" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="R69" s="15"/>
-      <c r="S69" s="15"/>
-      <c r="T69" s="15"/>
-    </row>
-    <row r="70" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="B70" s="15">
-        <v>0.05</v>
-      </c>
-      <c r="C70" s="15">
-        <v>3</v>
-      </c>
-      <c r="D70" s="15">
-        <v>100</v>
-      </c>
-      <c r="E70" s="15">
-        <v>0.3</v>
-      </c>
-      <c r="F70" s="15"/>
-      <c r="G70" s="15"/>
-      <c r="H70" s="15"/>
-      <c r="I70" s="15"/>
-      <c r="J70" s="15">
-        <v>100</v>
-      </c>
-      <c r="K70" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="L70" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="M70" s="15"/>
-      <c r="N70" s="15">
-        <v>50</v>
-      </c>
-      <c r="O70" s="15">
-        <v>100000</v>
-      </c>
-      <c r="P70" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q70" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="R70" s="15"/>
-      <c r="S70" s="15"/>
-      <c r="T70" s="15"/>
-    </row>
-    <row r="71" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="B71" s="15">
-        <v>0.05</v>
-      </c>
-      <c r="C71" s="15">
-        <v>3</v>
-      </c>
-      <c r="D71" s="15">
-        <v>100</v>
-      </c>
-      <c r="E71" s="15">
-        <v>0.3</v>
-      </c>
-      <c r="F71" s="15"/>
-      <c r="G71" s="15"/>
-      <c r="H71" s="15"/>
-      <c r="I71" s="15"/>
-      <c r="J71" s="15">
-        <v>100</v>
-      </c>
-      <c r="K71" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="L71" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="M71" s="15"/>
-      <c r="N71" s="15">
-        <v>50</v>
-      </c>
-      <c r="O71" s="15">
-        <v>100000</v>
-      </c>
-      <c r="P71" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q71" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="R71" s="15"/>
-      <c r="S71" s="15"/>
-      <c r="T71" s="15"/>
-    </row>
-    <row r="72" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="B72" s="15">
-        <v>0.05</v>
-      </c>
-      <c r="C72" s="15">
-        <v>3</v>
-      </c>
-      <c r="D72" s="15">
-        <v>100</v>
-      </c>
-      <c r="E72" s="15">
-        <v>0.3</v>
-      </c>
-      <c r="F72" s="15"/>
-      <c r="G72" s="15"/>
-      <c r="H72" s="15"/>
-      <c r="I72" s="15"/>
-      <c r="J72" s="15">
-        <v>100</v>
-      </c>
-      <c r="K72" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="L72" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="M72" s="15"/>
-      <c r="N72" s="15">
-        <v>50</v>
-      </c>
-      <c r="O72" s="15"/>
-      <c r="P72" s="15"/>
-      <c r="Q72" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="R72" s="15"/>
-      <c r="S72" s="15"/>
-      <c r="T72" s="15"/>
     </row>
     <row r="73" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A73" s="15" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="B73" s="15">
         <v>0.05</v>
@@ -3895,15 +3851,9 @@
       <c r="E73" s="15">
         <v>0.3</v>
       </c>
-      <c r="F73" s="15">
-        <v>100</v>
-      </c>
-      <c r="G73" s="15">
-        <v>0.3</v>
-      </c>
-      <c r="H73" s="15">
-        <v>0.5</v>
-      </c>
+      <c r="F73" s="15"/>
+      <c r="G73" s="15"/>
+      <c r="H73" s="15"/>
       <c r="I73" s="15"/>
       <c r="J73" s="15">
         <v>100</v>
@@ -3915,7 +3865,9 @@
         <v>18</v>
       </c>
       <c r="M73" s="15"/>
-      <c r="N73" s="15"/>
+      <c r="N73" s="15">
+        <v>50</v>
+      </c>
       <c r="O73" s="15">
         <v>100000</v>
       </c>
@@ -3931,7 +3883,7 @@
     </row>
     <row r="74" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A74" s="15" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="B74" s="15">
         <v>0.05</v>
@@ -3945,15 +3897,9 @@
       <c r="E74" s="15">
         <v>0.3</v>
       </c>
-      <c r="F74" s="15">
-        <v>100</v>
-      </c>
-      <c r="G74" s="15">
-        <v>0.3</v>
-      </c>
-      <c r="H74" s="15">
-        <v>0.5</v>
-      </c>
+      <c r="F74" s="15"/>
+      <c r="G74" s="15"/>
+      <c r="H74" s="15"/>
       <c r="I74" s="15"/>
       <c r="J74" s="15">
         <v>100</v>
@@ -3965,7 +3911,9 @@
         <v>18</v>
       </c>
       <c r="M74" s="15"/>
-      <c r="N74" s="15"/>
+      <c r="N74" s="15">
+        <v>50</v>
+      </c>
       <c r="O74" s="15">
         <v>100000</v>
       </c>
@@ -3981,7 +3929,7 @@
     </row>
     <row r="75" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A75" s="15" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="B75" s="15">
         <v>0.05</v>
@@ -3995,15 +3943,9 @@
       <c r="E75" s="15">
         <v>0.3</v>
       </c>
-      <c r="F75" s="15">
-        <v>100</v>
-      </c>
-      <c r="G75" s="15">
-        <v>0.3</v>
-      </c>
-      <c r="H75" s="15">
-        <v>0.5</v>
-      </c>
+      <c r="F75" s="15"/>
+      <c r="G75" s="15"/>
+      <c r="H75" s="15"/>
       <c r="I75" s="15"/>
       <c r="J75" s="15">
         <v>100</v>
@@ -4015,7 +3957,9 @@
         <v>18</v>
       </c>
       <c r="M75" s="15"/>
-      <c r="N75" s="15"/>
+      <c r="N75" s="15">
+        <v>50</v>
+      </c>
       <c r="O75" s="15">
         <v>100000</v>
       </c>
@@ -4031,7 +3975,7 @@
     </row>
     <row r="76" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" s="15" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="B76" s="15">
         <v>0.05</v>
@@ -4045,15 +3989,9 @@
       <c r="E76" s="15">
         <v>0.3</v>
       </c>
-      <c r="F76" s="15">
-        <v>100</v>
-      </c>
-      <c r="G76" s="15">
-        <v>0.3</v>
-      </c>
-      <c r="H76" s="15">
-        <v>0.5</v>
-      </c>
+      <c r="F76" s="15"/>
+      <c r="G76" s="15"/>
+      <c r="H76" s="15"/>
       <c r="I76" s="15"/>
       <c r="J76" s="15">
         <v>100</v>
@@ -4065,7 +4003,9 @@
         <v>18</v>
       </c>
       <c r="M76" s="15"/>
-      <c r="N76" s="15"/>
+      <c r="N76" s="15">
+        <v>50</v>
+      </c>
       <c r="O76" s="15">
         <v>100000</v>
       </c>
@@ -4081,7 +4021,7 @@
     </row>
     <row r="77" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A77" s="15" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="B77" s="15">
         <v>0.05</v>
@@ -4095,15 +4035,9 @@
       <c r="E77" s="15">
         <v>0.3</v>
       </c>
-      <c r="F77" s="15">
-        <v>100</v>
-      </c>
-      <c r="G77" s="15">
-        <v>0.3</v>
-      </c>
-      <c r="H77" s="15">
-        <v>0.5</v>
-      </c>
+      <c r="F77" s="15"/>
+      <c r="G77" s="15"/>
+      <c r="H77" s="15"/>
       <c r="I77" s="15"/>
       <c r="J77" s="15">
         <v>100</v>
@@ -4115,7 +4049,9 @@
         <v>17</v>
       </c>
       <c r="M77" s="15"/>
-      <c r="N77" s="15"/>
+      <c r="N77" s="15">
+        <v>50</v>
+      </c>
       <c r="O77" s="15">
         <v>100000</v>
       </c>
@@ -4131,7 +4067,7 @@
     </row>
     <row r="78" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A78" s="15" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="B78" s="15">
         <v>0.05</v>
@@ -4145,15 +4081,9 @@
       <c r="E78" s="15">
         <v>0.3</v>
       </c>
-      <c r="F78" s="15">
-        <v>100</v>
-      </c>
-      <c r="G78" s="15">
-        <v>0.3</v>
-      </c>
-      <c r="H78" s="15">
-        <v>0.5</v>
-      </c>
+      <c r="F78" s="15"/>
+      <c r="G78" s="15"/>
+      <c r="H78" s="15"/>
       <c r="I78" s="15"/>
       <c r="J78" s="15">
         <v>100</v>
@@ -4165,7 +4095,9 @@
         <v>17</v>
       </c>
       <c r="M78" s="15"/>
-      <c r="N78" s="15"/>
+      <c r="N78" s="15">
+        <v>50</v>
+      </c>
       <c r="O78" s="15"/>
       <c r="P78" s="15"/>
       <c r="Q78" s="15" t="b">
@@ -4177,137 +4109,179 @@
     </row>
     <row r="79" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A79" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B79" s="15">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="C79" s="15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D79" s="15">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="E79" s="15">
-        <v>0.4</v>
-      </c>
-      <c r="F79" s="15"/>
-      <c r="G79" s="15"/>
-      <c r="H79" s="15"/>
+        <v>0.3</v>
+      </c>
+      <c r="F79" s="15">
+        <v>100</v>
+      </c>
+      <c r="G79" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="H79" s="15">
+        <v>0.5</v>
+      </c>
       <c r="I79" s="15"/>
       <c r="J79" s="15">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="K79" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="L79" s="15"/>
+        <v>7</v>
+      </c>
+      <c r="L79" s="15" t="s">
+        <v>18</v>
+      </c>
       <c r="M79" s="15"/>
-      <c r="N79" s="15">
-        <v>200</v>
-      </c>
-      <c r="O79" s="15"/>
-      <c r="P79" s="15"/>
-      <c r="Q79" s="15"/>
+      <c r="N79" s="15"/>
+      <c r="O79" s="15">
+        <v>100000</v>
+      </c>
+      <c r="P79" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q79" s="15" t="b">
+        <v>1</v>
+      </c>
       <c r="R79" s="15"/>
       <c r="S79" s="15"/>
       <c r="T79" s="15"/>
     </row>
     <row r="80" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A80" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B80" s="15">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="C80" s="15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D80" s="15">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="E80" s="15">
-        <v>0.4</v>
-      </c>
-      <c r="F80" s="15"/>
-      <c r="G80" s="15"/>
-      <c r="H80" s="15"/>
+        <v>0.3</v>
+      </c>
+      <c r="F80" s="15">
+        <v>100</v>
+      </c>
+      <c r="G80" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="H80" s="15">
+        <v>0.5</v>
+      </c>
       <c r="I80" s="15"/>
       <c r="J80" s="15">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="K80" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="L80" s="15"/>
+        <v>7</v>
+      </c>
+      <c r="L80" s="15" t="s">
+        <v>18</v>
+      </c>
       <c r="M80" s="15"/>
-      <c r="N80" s="15">
-        <v>200</v>
-      </c>
-      <c r="O80" s="15"/>
-      <c r="P80" s="15"/>
-      <c r="Q80" s="15"/>
+      <c r="N80" s="15"/>
+      <c r="O80" s="15">
+        <v>100000</v>
+      </c>
+      <c r="P80" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q80" s="15" t="b">
+        <v>1</v>
+      </c>
       <c r="R80" s="15"/>
       <c r="S80" s="15"/>
       <c r="T80" s="15"/>
     </row>
     <row r="81" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A81" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B81" s="15">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="C81" s="15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D81" s="15">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="E81" s="15">
-        <v>0.4</v>
-      </c>
-      <c r="F81" s="15"/>
-      <c r="G81" s="15"/>
-      <c r="H81" s="15"/>
+        <v>0.3</v>
+      </c>
+      <c r="F81" s="15">
+        <v>100</v>
+      </c>
+      <c r="G81" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="H81" s="15">
+        <v>0.5</v>
+      </c>
       <c r="I81" s="15"/>
       <c r="J81" s="15">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="K81" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="L81" s="15"/>
+      <c r="L81" s="15" t="s">
+        <v>18</v>
+      </c>
       <c r="M81" s="15"/>
-      <c r="N81" s="15">
-        <v>200</v>
-      </c>
-      <c r="O81" s="15"/>
-      <c r="P81" s="15"/>
-      <c r="Q81" s="15"/>
+      <c r="N81" s="15"/>
+      <c r="O81" s="15">
+        <v>100000</v>
+      </c>
+      <c r="P81" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q81" s="15" t="b">
+        <v>1</v>
+      </c>
       <c r="R81" s="15"/>
       <c r="S81" s="15"/>
       <c r="T81" s="15"/>
     </row>
-    <row r="82" spans="1:20" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A82" s="15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B82" s="15">
         <v>0.05</v>
       </c>
       <c r="C82" s="15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D82" s="15">
         <v>100</v>
       </c>
       <c r="E82" s="15">
-        <v>0.2</v>
-      </c>
-      <c r="F82" s="15"/>
-      <c r="G82" s="15"/>
-      <c r="H82" s="15"/>
+        <v>0.3</v>
+      </c>
+      <c r="F82" s="15">
+        <v>100</v>
+      </c>
+      <c r="G82" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="H82" s="15">
+        <v>0.5</v>
+      </c>
       <c r="I82" s="15"/>
       <c r="J82" s="15">
         <v>100</v>
@@ -4315,23 +4289,277 @@
       <c r="K82" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="L82" s="15"/>
+      <c r="L82" s="15" t="s">
+        <v>18</v>
+      </c>
       <c r="M82" s="15"/>
-      <c r="N82" s="15">
+      <c r="N82" s="15"/>
+      <c r="O82" s="15">
+        <v>100000</v>
+      </c>
+      <c r="P82" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q82" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="R82" s="15"/>
+      <c r="S82" s="15"/>
+      <c r="T82" s="15"/>
+    </row>
+    <row r="83" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="O82" s="15">
-        <v>100000</v>
-      </c>
-      <c r="P82" s="15"/>
-      <c r="Q82" s="15"/>
-      <c r="R82" s="15">
+      <c r="B83" s="15">
+        <v>0.05</v>
+      </c>
+      <c r="C83" s="15">
+        <v>3</v>
+      </c>
+      <c r="D83" s="15">
+        <v>100</v>
+      </c>
+      <c r="E83" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="F83" s="15">
+        <v>100</v>
+      </c>
+      <c r="G83" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="H83" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="I83" s="15"/>
+      <c r="J83" s="15">
+        <v>100</v>
+      </c>
+      <c r="K83" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="L83" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="M83" s="15"/>
+      <c r="N83" s="15"/>
+      <c r="O83" s="15">
+        <v>100000</v>
+      </c>
+      <c r="P83" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q83" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="R83" s="15"/>
+      <c r="S83" s="15"/>
+      <c r="T83" s="15"/>
+    </row>
+    <row r="84" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B84" s="15">
+        <v>0.05</v>
+      </c>
+      <c r="C84" s="15">
+        <v>3</v>
+      </c>
+      <c r="D84" s="15">
+        <v>100</v>
+      </c>
+      <c r="E84" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="F84" s="15">
+        <v>100</v>
+      </c>
+      <c r="G84" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="H84" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="I84" s="15"/>
+      <c r="J84" s="15">
+        <v>100</v>
+      </c>
+      <c r="K84" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="L84" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="M84" s="15"/>
+      <c r="N84" s="15"/>
+      <c r="O84" s="15"/>
+      <c r="P84" s="15"/>
+      <c r="Q84" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="R84" s="15"/>
+      <c r="S84" s="15"/>
+      <c r="T84" s="15"/>
+    </row>
+    <row r="85" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B85" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="C85" s="15">
+        <v>2</v>
+      </c>
+      <c r="D85" s="15">
+        <v>50</v>
+      </c>
+      <c r="E85" s="15">
+        <v>0.4</v>
+      </c>
+      <c r="F85" s="15"/>
+      <c r="G85" s="15"/>
+      <c r="H85" s="15"/>
+      <c r="I85" s="15"/>
+      <c r="J85" s="15">
+        <v>40</v>
+      </c>
+      <c r="K85" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="L85" s="15"/>
+      <c r="M85" s="15"/>
+      <c r="N85" s="15">
+        <v>200</v>
+      </c>
+      <c r="O85" s="15"/>
+      <c r="P85" s="15"/>
+      <c r="Q85" s="15"/>
+      <c r="R85" s="15"/>
+      <c r="S85" s="15"/>
+      <c r="T85" s="15"/>
+    </row>
+    <row r="86" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B86" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="C86" s="15">
+        <v>2</v>
+      </c>
+      <c r="D86" s="15">
+        <v>50</v>
+      </c>
+      <c r="E86" s="15">
+        <v>0.4</v>
+      </c>
+      <c r="F86" s="15"/>
+      <c r="G86" s="15"/>
+      <c r="H86" s="15"/>
+      <c r="I86" s="15"/>
+      <c r="J86" s="15">
+        <v>50</v>
+      </c>
+      <c r="K86" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="L86" s="15"/>
+      <c r="M86" s="15"/>
+      <c r="N86" s="15">
+        <v>200</v>
+      </c>
+      <c r="O86" s="15"/>
+      <c r="P86" s="15"/>
+      <c r="Q86" s="15"/>
+      <c r="R86" s="15"/>
+      <c r="S86" s="15"/>
+      <c r="T86" s="15"/>
+    </row>
+    <row r="87" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B87" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="C87" s="15">
+        <v>2</v>
+      </c>
+      <c r="D87" s="15">
+        <v>50</v>
+      </c>
+      <c r="E87" s="15">
+        <v>0.4</v>
+      </c>
+      <c r="F87" s="15"/>
+      <c r="G87" s="15"/>
+      <c r="H87" s="15"/>
+      <c r="I87" s="15"/>
+      <c r="J87" s="15">
+        <v>70</v>
+      </c>
+      <c r="K87" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="L87" s="15"/>
+      <c r="M87" s="15"/>
+      <c r="N87" s="15">
+        <v>200</v>
+      </c>
+      <c r="O87" s="15"/>
+      <c r="P87" s="15"/>
+      <c r="Q87" s="15"/>
+      <c r="R87" s="15"/>
+      <c r="S87" s="15"/>
+      <c r="T87" s="15"/>
+    </row>
+    <row r="88" spans="1:20" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B88" s="15">
+        <v>0.05</v>
+      </c>
+      <c r="C88" s="15">
+        <v>2</v>
+      </c>
+      <c r="D88" s="15">
+        <v>100</v>
+      </c>
+      <c r="E88" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="F88" s="15"/>
+      <c r="G88" s="15"/>
+      <c r="H88" s="15"/>
+      <c r="I88" s="15"/>
+      <c r="J88" s="15">
+        <v>100</v>
+      </c>
+      <c r="K88" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="L88" s="15"/>
+      <c r="M88" s="15"/>
+      <c r="N88" s="15">
+        <v>24</v>
+      </c>
+      <c r="O88" s="15">
+        <v>100000</v>
+      </c>
+      <c r="P88" s="15"/>
+      <c r="Q88" s="15"/>
+      <c r="R88" s="15">
         <v>80</v>
       </c>
-      <c r="S82" s="15">
+      <c r="S88" s="15">
         <v>125</v>
       </c>
-      <c r="T82" s="15">
+      <c r="T88" s="15">
         <v>1.5</v>
       </c>
     </row>

</xml_diff>